<commit_message>
Revert "Merge branch 'main' into Db_system"
This reverts commit 1b492ebba66beb658ed21d970171b740a145b2ae, reversing
changes made to a57a5ec0377ce404a69a2277e22efeb00833c6dc.
</commit_message>
<xml_diff>
--- a/OOP/src/assets/Book1.xlsx
+++ b/OOP/src/assets/Book1.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2808" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1482" uniqueCount="229">
   <si>
     <t/>
   </si>
@@ -708,12 +708,6 @@
   </si>
   <si>
     <t>63070024</t>
-  </si>
-  <si>
-    <t>ปฐมกานต์ สุวรรน้อย</t>
-  </si>
-  <si>
-    <t>ใคร ไม่รู้</t>
   </si>
 </sst>
 </file>
@@ -1172,19 +1166,19 @@
         <v>8</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>229</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>6</v>
+      <c r="F2" s="0">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
@@ -1192,7 +1186,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>230</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>0</v>
@@ -1203,8 +1197,8 @@
       <c r="E3" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>6</v>
+      <c r="F3" s="0">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
@@ -3355,9 +3349,6 @@
       <c r="E86" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="F86" t="s" s="0">
-        <v>0</v>
-      </c>
       <c r="G86" t="s" s="0">
         <v>0</v>
       </c>
@@ -3378,12 +3369,6 @@
       <c r="D87" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E87" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F87" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="88" spans="1:8" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="2" t="s">
@@ -3398,12 +3383,6 @@
       <c r="D88" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E88" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F88" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="89" spans="1:8" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="2" t="s">
@@ -3418,12 +3397,6 @@
       <c r="D89" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E89" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F89" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="90" spans="1:8" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="2" t="s">
@@ -3438,12 +3411,6 @@
       <c r="D90" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E90" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F90" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="91" spans="1:8" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="2" t="s">
@@ -3458,12 +3425,6 @@
       <c r="D91" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E91" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F91" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="92" spans="1:8" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="2" t="s">
@@ -3478,12 +3439,6 @@
       <c r="D92" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E92" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F92" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="93" spans="1:8" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="2" t="s">
@@ -3498,12 +3453,6 @@
       <c r="D93" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E93" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F93" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="94" spans="1:8" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="2" t="s">
@@ -3518,12 +3467,6 @@
       <c r="D94" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E94" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F94" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="95" spans="1:8" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="2" t="s">
@@ -3538,12 +3481,6 @@
       <c r="D95" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E95" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F95" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="96" spans="1:8" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="2" t="s">
@@ -3558,12 +3495,6 @@
       <c r="D96" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E96" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F96" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="97" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="2" t="s">
@@ -3578,12 +3509,6 @@
       <c r="D97" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E97" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F97" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="98" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="2" t="s">
@@ -3598,12 +3523,6 @@
       <c r="D98" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E98" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F98" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="99" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="2" t="s">
@@ -3618,12 +3537,6 @@
       <c r="D99" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E99" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F99" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="100" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="2" t="s">
@@ -3638,12 +3551,6 @@
       <c r="D100" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E100" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F100" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="101" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="2" t="s">
@@ -3658,12 +3565,6 @@
       <c r="D101" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E101" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F101" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="102" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="2" t="s">
@@ -3678,12 +3579,6 @@
       <c r="D102" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E102" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F102" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="103" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="2" t="s">
@@ -3698,12 +3593,6 @@
       <c r="D103" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E103" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F103" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="104" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="2" t="s">
@@ -3718,12 +3607,6 @@
       <c r="D104" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E104" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F104" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="105" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="2" t="s">
@@ -3738,12 +3621,6 @@
       <c r="D105" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E105" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F105" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="106" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="2" t="s">
@@ -3758,12 +3635,6 @@
       <c r="D106" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E106" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F106" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="107" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="2" t="s">
@@ -3778,12 +3649,6 @@
       <c r="D107" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E107" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F107" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="108" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="2" t="s">
@@ -3798,12 +3663,6 @@
       <c r="D108" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E108" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F108" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="109" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="2" t="s">
@@ -3818,12 +3677,6 @@
       <c r="D109" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E109" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F109" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="110" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="2" t="s">
@@ -3838,12 +3691,6 @@
       <c r="D110" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E110" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F110" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="111" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="2" t="s">
@@ -3858,12 +3705,6 @@
       <c r="D111" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E111" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F111" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="112" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="2" t="s">
@@ -3878,12 +3719,6 @@
       <c r="D112" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E112" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F112" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="113" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="2" t="s">
@@ -3898,12 +3733,6 @@
       <c r="D113" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E113" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F113" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="114" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="2" t="s">
@@ -3918,12 +3747,6 @@
       <c r="D114" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E114" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F114" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="115" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="2" t="s">
@@ -3938,12 +3761,6 @@
       <c r="D115" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E115" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F115" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="116" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="2" t="s">
@@ -3958,12 +3775,6 @@
       <c r="D116" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E116" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F116" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="117" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="2" t="s">
@@ -3978,12 +3789,6 @@
       <c r="D117" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E117" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F117" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="118" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="2" t="s">
@@ -3998,12 +3803,6 @@
       <c r="D118" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E118" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F118" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="119" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="2" t="s">
@@ -4018,12 +3817,6 @@
       <c r="D119" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E119" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F119" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="120" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="2" t="s">
@@ -4038,12 +3831,6 @@
       <c r="D120" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E120" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F120" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="121" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="2" t="s">
@@ -4058,12 +3845,6 @@
       <c r="D121" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E121" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F121" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="122" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="2" t="s">
@@ -4078,12 +3859,6 @@
       <c r="D122" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E122" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F122" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="123" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="2" t="s">
@@ -4098,12 +3873,6 @@
       <c r="D123" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E123" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F123" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="124" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="2" t="s">
@@ -4118,12 +3887,6 @@
       <c r="D124" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E124" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F124" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="125" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="2" t="s">
@@ -4138,12 +3901,6 @@
       <c r="D125" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E125" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F125" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="126" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="2" t="s">
@@ -4158,12 +3915,6 @@
       <c r="D126" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E126" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F126" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="127" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="2" t="s">
@@ -4178,12 +3929,6 @@
       <c r="D127" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E127" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F127" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="128" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="2" t="s">
@@ -4198,12 +3943,6 @@
       <c r="D128" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E128" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F128" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="129" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="2" t="s">
@@ -4218,12 +3957,6 @@
       <c r="D129" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E129" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F129" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="130" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="2" t="s">
@@ -4238,12 +3971,6 @@
       <c r="D130" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E130" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F130" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="131" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="2" t="s">
@@ -4258,12 +3985,6 @@
       <c r="D131" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E131" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F131" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="132" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="2" t="s">
@@ -4278,12 +3999,6 @@
       <c r="D132" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E132" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F132" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="133" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="2" t="s">
@@ -4298,12 +4013,6 @@
       <c r="D133" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E133" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F133" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="134" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="2" t="s">
@@ -4318,12 +4027,6 @@
       <c r="D134" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E134" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F134" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="135" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="2" t="s">
@@ -4338,12 +4041,6 @@
       <c r="D135" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E135" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F135" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="136" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="2" t="s">
@@ -4358,12 +4055,6 @@
       <c r="D136" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E136" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F136" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="137" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="2" t="s">
@@ -4378,12 +4069,6 @@
       <c r="D137" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E137" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F137" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="138" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="2" t="s">
@@ -4398,12 +4083,6 @@
       <c r="D138" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E138" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F138" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="139" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="2" t="s">
@@ -4418,12 +4097,6 @@
       <c r="D139" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E139" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F139" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="140" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="2" t="s">
@@ -4438,12 +4111,6 @@
       <c r="D140" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E140" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F140" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="141" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="2" t="s">
@@ -4458,12 +4125,6 @@
       <c r="D141" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E141" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F141" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="142" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="2" t="s">
@@ -4478,12 +4139,6 @@
       <c r="D142" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E142" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F142" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="143" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="2" t="s">
@@ -4498,12 +4153,6 @@
       <c r="D143" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E143" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F143" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="144" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="2" t="s">
@@ -4518,12 +4167,6 @@
       <c r="D144" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E144" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F144" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="145" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="2" t="s">
@@ -4538,12 +4181,6 @@
       <c r="D145" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E145" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F145" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="146" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="2" t="s">
@@ -4558,12 +4195,6 @@
       <c r="D146" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E146" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F146" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="147" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="2" t="s">
@@ -4578,12 +4209,6 @@
       <c r="D147" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E147" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F147" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="148" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="2" t="s">
@@ -4598,12 +4223,6 @@
       <c r="D148" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E148" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F148" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="149" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" s="2" t="s">
@@ -4618,12 +4237,6 @@
       <c r="D149" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E149" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F149" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="150" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="2" t="s">
@@ -4638,12 +4251,6 @@
       <c r="D150" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E150" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F150" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="151" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="2" t="s">
@@ -4658,12 +4265,6 @@
       <c r="D151" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E151" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F151" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="152" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="2" t="s">
@@ -4678,12 +4279,6 @@
       <c r="D152" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E152" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F152" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="153" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="2" t="s">
@@ -4698,12 +4293,6 @@
       <c r="D153" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E153" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F153" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="154" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" s="2" t="s">
@@ -4718,12 +4307,6 @@
       <c r="D154" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E154" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F154" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="155" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="2" t="s">
@@ -4738,12 +4321,6 @@
       <c r="D155" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E155" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F155" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="156" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="2" t="s">
@@ -4758,12 +4335,6 @@
       <c r="D156" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E156" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F156" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="157" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="2" t="s">
@@ -4778,12 +4349,6 @@
       <c r="D157" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E157" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F157" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="158" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" s="2" t="s">
@@ -4798,12 +4363,6 @@
       <c r="D158" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E158" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F158" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="159" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" s="2" t="s">
@@ -4818,12 +4377,6 @@
       <c r="D159" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E159" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F159" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="160" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" s="2" t="s">
@@ -4838,12 +4391,6 @@
       <c r="D160" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E160" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F160" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="161" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" s="2" t="s">
@@ -4858,12 +4405,6 @@
       <c r="D161" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E161" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F161" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="162" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" s="2" t="s">
@@ -4878,12 +4419,6 @@
       <c r="D162" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E162" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F162" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="163" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" s="2" t="s">
@@ -4898,12 +4433,6 @@
       <c r="D163" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E163" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F163" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="164" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" s="2" t="s">
@@ -4918,12 +4447,6 @@
       <c r="D164" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E164" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F164" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="165" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" s="2" t="s">
@@ -4938,12 +4461,6 @@
       <c r="D165" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E165" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F165" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="166" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" s="2" t="s">
@@ -4958,12 +4475,6 @@
       <c r="D166" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E166" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F166" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="167" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" s="2" t="s">
@@ -4978,12 +4489,6 @@
       <c r="D167" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E167" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F167" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="168" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="2" t="s">
@@ -4998,12 +4503,6 @@
       <c r="D168" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E168" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F168" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="169" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" s="2" t="s">
@@ -5018,12 +4517,6 @@
       <c r="D169" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E169" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F169" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="170" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" s="2" t="s">
@@ -5038,12 +4531,6 @@
       <c r="D170" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E170" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F170" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="171" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="2" t="s">
@@ -5058,12 +4545,6 @@
       <c r="D171" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E171" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F171" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="172" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" s="2" t="s">
@@ -5078,12 +4559,6 @@
       <c r="D172" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E172" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F172" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="173" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" s="2" t="s">
@@ -5098,12 +4573,6 @@
       <c r="D173" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E173" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F173" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="174" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" s="2" t="s">
@@ -5118,12 +4587,6 @@
       <c r="D174" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E174" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F174" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="175" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" s="2" t="s">
@@ -5138,12 +4601,6 @@
       <c r="D175" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E175" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F175" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="176" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" s="2" t="s">
@@ -5158,12 +4615,6 @@
       <c r="D176" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E176" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F176" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="177" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" s="2" t="s">
@@ -5178,12 +4629,6 @@
       <c r="D177" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E177" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F177" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="178" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" s="2" t="s">
@@ -5198,12 +4643,6 @@
       <c r="D178" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E178" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F178" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="179" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" s="2" t="s">
@@ -5218,12 +4657,6 @@
       <c r="D179" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E179" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F179" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="180" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" s="2" t="s">
@@ -5238,12 +4671,6 @@
       <c r="D180" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E180" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F180" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="181" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" s="2" t="s">
@@ -5258,12 +4685,6 @@
       <c r="D181" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E181" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F181" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="182" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" s="2" t="s">
@@ -5278,12 +4699,6 @@
       <c r="D182" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E182" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F182" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="183" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" s="2" t="s">
@@ -5298,12 +4713,6 @@
       <c r="D183" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E183" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F183" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="184" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" s="2" t="s">
@@ -5318,12 +4727,6 @@
       <c r="D184" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E184" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F184" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="185" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" s="2" t="s">
@@ -5338,12 +4741,6 @@
       <c r="D185" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E185" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F185" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="186" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" s="2" t="s">
@@ -5358,12 +4755,6 @@
       <c r="D186" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E186" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F186" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="187" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" s="2" t="s">
@@ -5378,12 +4769,6 @@
       <c r="D187" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E187" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F187" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="188" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" s="2" t="s">
@@ -5398,12 +4783,6 @@
       <c r="D188" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E188" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F188" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="189" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" s="2" t="s">
@@ -5418,12 +4797,6 @@
       <c r="D189" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E189" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F189" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="190" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A190" s="2" t="s">
@@ -5438,12 +4811,6 @@
       <c r="D190" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E190" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F190" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="191" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A191" s="2" t="s">
@@ -5458,12 +4825,6 @@
       <c r="D191" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E191" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F191" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="192" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A192" s="2" t="s">
@@ -5478,12 +4839,6 @@
       <c r="D192" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E192" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F192" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="193" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A193" s="2" t="s">
@@ -5498,12 +4853,6 @@
       <c r="D193" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E193" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F193" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="194" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A194" s="2" t="s">
@@ -5518,12 +4867,6 @@
       <c r="D194" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E194" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F194" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="195" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A195" s="2" t="s">
@@ -5538,12 +4881,6 @@
       <c r="D195" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E195" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F195" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="196" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A196" s="2" t="s">
@@ -5558,12 +4895,6 @@
       <c r="D196" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E196" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F196" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="197" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A197" s="2" t="s">
@@ -5578,12 +4909,6 @@
       <c r="D197" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E197" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F197" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="198" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A198" s="2" t="s">
@@ -5598,12 +4923,6 @@
       <c r="D198" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E198" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F198" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="199" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A199" s="2" t="s">
@@ -5618,12 +4937,6 @@
       <c r="D199" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E199" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F199" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="200" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A200" s="2" t="s">
@@ -5638,12 +4951,6 @@
       <c r="D200" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E200" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F200" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="201" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A201" s="2" t="s">
@@ -5658,12 +4965,6 @@
       <c r="D201" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E201" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F201" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="202" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A202" s="2" t="s">
@@ -5678,12 +4979,6 @@
       <c r="D202" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E202" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F202" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="203" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A203" s="2" t="s">
@@ -5698,12 +4993,6 @@
       <c r="D203" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E203" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F203" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="204" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A204" s="2" t="s">
@@ -5718,12 +5007,6 @@
       <c r="D204" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E204" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F204" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="205" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A205" s="2" t="s">
@@ -5738,12 +5021,6 @@
       <c r="D205" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E205" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F205" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="206" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A206" s="2" t="s">
@@ -5758,12 +5035,6 @@
       <c r="D206" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E206" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F206" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="207" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A207" s="2" t="s">
@@ -5778,12 +5049,6 @@
       <c r="D207" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E207" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F207" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="208" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A208" s="2" t="s">
@@ -5798,12 +5063,6 @@
       <c r="D208" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E208" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F208" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="209" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A209" s="2" t="s">
@@ -5818,12 +5077,6 @@
       <c r="D209" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E209" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F209" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="210" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A210" s="2" t="s">
@@ -5838,12 +5091,6 @@
       <c r="D210" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E210" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F210" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="211" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A211" s="2" t="s">
@@ -5858,12 +5105,6 @@
       <c r="D211" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E211" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F211" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="212" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A212" s="2" t="s">
@@ -5878,12 +5119,6 @@
       <c r="D212" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E212" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F212" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="213" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A213" s="2" t="s">
@@ -5898,12 +5133,6 @@
       <c r="D213" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E213" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F213" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="214" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A214" s="2" t="s">
@@ -5918,12 +5147,6 @@
       <c r="D214" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E214" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F214" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="215" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A215" s="2" t="s">
@@ -5938,12 +5161,6 @@
       <c r="D215" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E215" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F215" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="216" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A216" s="2" t="s">
@@ -5958,12 +5175,6 @@
       <c r="D216" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E216" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F216" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="217" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A217" s="2" t="s">
@@ -5978,12 +5189,6 @@
       <c r="D217" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E217" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F217" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="218" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A218" s="2" t="s">
@@ -5998,12 +5203,6 @@
       <c r="D218" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E218" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F218" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="219" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A219" s="2" t="s">
@@ -6018,12 +5217,6 @@
       <c r="D219" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E219" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F219" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="220" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A220" s="2" t="s">
@@ -6038,12 +5231,6 @@
       <c r="D220" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E220" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F220" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="221" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A221" s="2" t="s">
@@ -6058,12 +5245,6 @@
       <c r="D221" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E221" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F221" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="222" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A222" s="2" t="s">
@@ -6076,12 +5257,6 @@
         <v>0</v>
       </c>
       <c r="D222" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E222" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F222" t="s" s="0">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Merge branch 'main' into New_Db_system"
This reverts commit e86c42a50442afa3383f852649df0bdb1927e675, reversing
changes made to 6d2de5538246e4c10b982006c8097eba3d586dd3.
</commit_message>
<xml_diff>
--- a/OOP/src/assets/Book1.xlsx
+++ b/OOP/src/assets/Book1.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2808" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1482" uniqueCount="229">
   <si>
     <t/>
   </si>
@@ -708,12 +708,6 @@
   </si>
   <si>
     <t>63070024</t>
-  </si>
-  <si>
-    <t>ปฐมกานต์ สุวรรน้อย</t>
-  </si>
-  <si>
-    <t>ใคร ไม่รู้</t>
   </si>
 </sst>
 </file>
@@ -1172,19 +1166,19 @@
         <v>8</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>229</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>6</v>
+      <c r="F2" s="0">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
@@ -1192,7 +1186,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>230</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>0</v>
@@ -1203,8 +1197,8 @@
       <c r="E3" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>6</v>
+      <c r="F3" s="0">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
@@ -3355,9 +3349,6 @@
       <c r="E86" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="F86" t="s" s="0">
-        <v>0</v>
-      </c>
       <c r="G86" t="s" s="0">
         <v>0</v>
       </c>
@@ -3378,12 +3369,6 @@
       <c r="D87" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E87" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F87" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="88" spans="1:8" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="2" t="s">
@@ -3398,12 +3383,6 @@
       <c r="D88" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E88" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F88" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="89" spans="1:8" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="2" t="s">
@@ -3418,12 +3397,6 @@
       <c r="D89" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E89" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F89" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="90" spans="1:8" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="2" t="s">
@@ -3438,12 +3411,6 @@
       <c r="D90" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E90" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F90" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="91" spans="1:8" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="2" t="s">
@@ -3458,12 +3425,6 @@
       <c r="D91" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E91" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F91" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="92" spans="1:8" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="2" t="s">
@@ -3478,12 +3439,6 @@
       <c r="D92" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E92" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F92" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="93" spans="1:8" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="2" t="s">
@@ -3498,12 +3453,6 @@
       <c r="D93" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E93" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F93" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="94" spans="1:8" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="2" t="s">
@@ -3518,12 +3467,6 @@
       <c r="D94" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E94" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F94" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="95" spans="1:8" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="2" t="s">
@@ -3538,12 +3481,6 @@
       <c r="D95" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E95" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F95" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="96" spans="1:8" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="2" t="s">
@@ -3558,12 +3495,6 @@
       <c r="D96" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E96" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F96" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="97" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="2" t="s">
@@ -3578,12 +3509,6 @@
       <c r="D97" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E97" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F97" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="98" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="2" t="s">
@@ -3598,12 +3523,6 @@
       <c r="D98" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E98" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F98" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="99" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="2" t="s">
@@ -3618,12 +3537,6 @@
       <c r="D99" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E99" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F99" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="100" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="2" t="s">
@@ -3638,12 +3551,6 @@
       <c r="D100" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E100" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F100" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="101" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="2" t="s">
@@ -3658,12 +3565,6 @@
       <c r="D101" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E101" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F101" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="102" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="2" t="s">
@@ -3678,12 +3579,6 @@
       <c r="D102" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E102" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F102" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="103" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="2" t="s">
@@ -3698,12 +3593,6 @@
       <c r="D103" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E103" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F103" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="104" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="2" t="s">
@@ -3718,12 +3607,6 @@
       <c r="D104" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E104" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F104" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="105" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="2" t="s">
@@ -3738,12 +3621,6 @@
       <c r="D105" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E105" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F105" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="106" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="2" t="s">
@@ -3758,12 +3635,6 @@
       <c r="D106" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E106" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F106" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="107" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="2" t="s">
@@ -3778,12 +3649,6 @@
       <c r="D107" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E107" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F107" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="108" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="2" t="s">
@@ -3798,12 +3663,6 @@
       <c r="D108" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E108" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F108" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="109" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="2" t="s">
@@ -3818,12 +3677,6 @@
       <c r="D109" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E109" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F109" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="110" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="2" t="s">
@@ -3838,12 +3691,6 @@
       <c r="D110" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E110" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F110" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="111" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="2" t="s">
@@ -3858,12 +3705,6 @@
       <c r="D111" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E111" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F111" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="112" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="2" t="s">
@@ -3878,12 +3719,6 @@
       <c r="D112" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E112" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F112" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="113" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="2" t="s">
@@ -3898,12 +3733,6 @@
       <c r="D113" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E113" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F113" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="114" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="2" t="s">
@@ -3918,12 +3747,6 @@
       <c r="D114" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E114" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F114" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="115" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="2" t="s">
@@ -3938,12 +3761,6 @@
       <c r="D115" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E115" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F115" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="116" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="2" t="s">
@@ -3958,12 +3775,6 @@
       <c r="D116" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E116" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F116" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="117" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="2" t="s">
@@ -3978,12 +3789,6 @@
       <c r="D117" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E117" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F117" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="118" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="2" t="s">
@@ -3998,12 +3803,6 @@
       <c r="D118" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E118" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F118" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="119" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="2" t="s">
@@ -4018,12 +3817,6 @@
       <c r="D119" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E119" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F119" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="120" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="2" t="s">
@@ -4038,12 +3831,6 @@
       <c r="D120" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E120" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F120" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="121" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="2" t="s">
@@ -4058,12 +3845,6 @@
       <c r="D121" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E121" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F121" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="122" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="2" t="s">
@@ -4078,12 +3859,6 @@
       <c r="D122" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E122" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F122" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="123" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="2" t="s">
@@ -4098,12 +3873,6 @@
       <c r="D123" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E123" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F123" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="124" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="2" t="s">
@@ -4118,12 +3887,6 @@
       <c r="D124" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E124" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F124" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="125" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="2" t="s">
@@ -4138,12 +3901,6 @@
       <c r="D125" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E125" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F125" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="126" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="2" t="s">
@@ -4158,12 +3915,6 @@
       <c r="D126" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E126" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F126" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="127" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="2" t="s">
@@ -4178,12 +3929,6 @@
       <c r="D127" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E127" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F127" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="128" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="2" t="s">
@@ -4198,12 +3943,6 @@
       <c r="D128" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E128" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F128" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="129" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="2" t="s">
@@ -4218,12 +3957,6 @@
       <c r="D129" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E129" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F129" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="130" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="2" t="s">
@@ -4238,12 +3971,6 @@
       <c r="D130" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E130" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F130" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="131" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="2" t="s">
@@ -4258,12 +3985,6 @@
       <c r="D131" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E131" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F131" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="132" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="2" t="s">
@@ -4278,12 +3999,6 @@
       <c r="D132" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E132" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F132" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="133" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="2" t="s">
@@ -4298,12 +4013,6 @@
       <c r="D133" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E133" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F133" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="134" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="2" t="s">
@@ -4318,12 +4027,6 @@
       <c r="D134" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E134" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F134" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="135" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="2" t="s">
@@ -4338,12 +4041,6 @@
       <c r="D135" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E135" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F135" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="136" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="2" t="s">
@@ -4358,12 +4055,6 @@
       <c r="D136" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E136" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F136" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="137" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="2" t="s">
@@ -4378,12 +4069,6 @@
       <c r="D137" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E137" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F137" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="138" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="2" t="s">
@@ -4398,12 +4083,6 @@
       <c r="D138" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E138" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F138" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="139" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="2" t="s">
@@ -4418,12 +4097,6 @@
       <c r="D139" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E139" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F139" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="140" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="2" t="s">
@@ -4438,12 +4111,6 @@
       <c r="D140" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E140" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F140" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="141" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="2" t="s">
@@ -4458,12 +4125,6 @@
       <c r="D141" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E141" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F141" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="142" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="2" t="s">
@@ -4478,12 +4139,6 @@
       <c r="D142" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E142" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F142" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="143" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="2" t="s">
@@ -4498,12 +4153,6 @@
       <c r="D143" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E143" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F143" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="144" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="2" t="s">
@@ -4518,12 +4167,6 @@
       <c r="D144" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E144" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F144" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="145" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="2" t="s">
@@ -4538,12 +4181,6 @@
       <c r="D145" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E145" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F145" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="146" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="2" t="s">
@@ -4558,12 +4195,6 @@
       <c r="D146" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E146" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F146" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="147" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="2" t="s">
@@ -4578,12 +4209,6 @@
       <c r="D147" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E147" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F147" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="148" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="2" t="s">
@@ -4598,12 +4223,6 @@
       <c r="D148" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E148" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F148" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="149" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" s="2" t="s">
@@ -4618,12 +4237,6 @@
       <c r="D149" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E149" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F149" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="150" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="2" t="s">
@@ -4638,12 +4251,6 @@
       <c r="D150" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E150" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F150" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="151" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="2" t="s">
@@ -4658,12 +4265,6 @@
       <c r="D151" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E151" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F151" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="152" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="2" t="s">
@@ -4678,12 +4279,6 @@
       <c r="D152" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E152" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F152" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="153" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="2" t="s">
@@ -4698,12 +4293,6 @@
       <c r="D153" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E153" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F153" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="154" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" s="2" t="s">
@@ -4718,12 +4307,6 @@
       <c r="D154" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E154" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F154" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="155" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="2" t="s">
@@ -4738,12 +4321,6 @@
       <c r="D155" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E155" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F155" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="156" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="2" t="s">
@@ -4758,12 +4335,6 @@
       <c r="D156" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E156" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F156" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="157" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="2" t="s">
@@ -4778,12 +4349,6 @@
       <c r="D157" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E157" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F157" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="158" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" s="2" t="s">
@@ -4798,12 +4363,6 @@
       <c r="D158" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E158" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F158" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="159" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" s="2" t="s">
@@ -4818,12 +4377,6 @@
       <c r="D159" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E159" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F159" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="160" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" s="2" t="s">
@@ -4838,12 +4391,6 @@
       <c r="D160" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E160" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F160" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="161" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" s="2" t="s">
@@ -4858,12 +4405,6 @@
       <c r="D161" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E161" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F161" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="162" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" s="2" t="s">
@@ -4878,12 +4419,6 @@
       <c r="D162" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E162" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F162" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="163" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" s="2" t="s">
@@ -4898,12 +4433,6 @@
       <c r="D163" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E163" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F163" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="164" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" s="2" t="s">
@@ -4918,12 +4447,6 @@
       <c r="D164" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E164" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F164" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="165" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" s="2" t="s">
@@ -4938,12 +4461,6 @@
       <c r="D165" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E165" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F165" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="166" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" s="2" t="s">
@@ -4958,12 +4475,6 @@
       <c r="D166" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E166" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F166" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="167" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" s="2" t="s">
@@ -4978,12 +4489,6 @@
       <c r="D167" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E167" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F167" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="168" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="2" t="s">
@@ -4998,12 +4503,6 @@
       <c r="D168" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E168" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F168" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="169" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" s="2" t="s">
@@ -5018,12 +4517,6 @@
       <c r="D169" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E169" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F169" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="170" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" s="2" t="s">
@@ -5038,12 +4531,6 @@
       <c r="D170" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E170" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F170" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="171" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="2" t="s">
@@ -5058,12 +4545,6 @@
       <c r="D171" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E171" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F171" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="172" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" s="2" t="s">
@@ -5078,12 +4559,6 @@
       <c r="D172" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E172" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F172" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="173" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" s="2" t="s">
@@ -5098,12 +4573,6 @@
       <c r="D173" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E173" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F173" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="174" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" s="2" t="s">
@@ -5118,12 +4587,6 @@
       <c r="D174" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E174" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F174" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="175" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" s="2" t="s">
@@ -5138,12 +4601,6 @@
       <c r="D175" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E175" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F175" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="176" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" s="2" t="s">
@@ -5158,12 +4615,6 @@
       <c r="D176" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E176" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F176" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="177" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" s="2" t="s">
@@ -5178,12 +4629,6 @@
       <c r="D177" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E177" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F177" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="178" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" s="2" t="s">
@@ -5198,12 +4643,6 @@
       <c r="D178" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E178" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F178" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="179" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" s="2" t="s">
@@ -5218,12 +4657,6 @@
       <c r="D179" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E179" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F179" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="180" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" s="2" t="s">
@@ -5238,12 +4671,6 @@
       <c r="D180" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E180" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F180" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="181" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" s="2" t="s">
@@ -5258,12 +4685,6 @@
       <c r="D181" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E181" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F181" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="182" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" s="2" t="s">
@@ -5278,12 +4699,6 @@
       <c r="D182" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E182" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F182" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="183" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" s="2" t="s">
@@ -5298,12 +4713,6 @@
       <c r="D183" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E183" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F183" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="184" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" s="2" t="s">
@@ -5318,12 +4727,6 @@
       <c r="D184" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E184" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F184" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="185" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" s="2" t="s">
@@ -5338,12 +4741,6 @@
       <c r="D185" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E185" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F185" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="186" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" s="2" t="s">
@@ -5358,12 +4755,6 @@
       <c r="D186" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E186" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F186" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="187" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" s="2" t="s">
@@ -5378,12 +4769,6 @@
       <c r="D187" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E187" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F187" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="188" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" s="2" t="s">
@@ -5398,12 +4783,6 @@
       <c r="D188" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E188" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F188" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="189" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" s="2" t="s">
@@ -5418,12 +4797,6 @@
       <c r="D189" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E189" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F189" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="190" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A190" s="2" t="s">
@@ -5438,12 +4811,6 @@
       <c r="D190" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E190" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F190" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="191" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A191" s="2" t="s">
@@ -5458,12 +4825,6 @@
       <c r="D191" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E191" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F191" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="192" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A192" s="2" t="s">
@@ -5478,12 +4839,6 @@
       <c r="D192" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E192" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F192" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="193" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A193" s="2" t="s">
@@ -5498,12 +4853,6 @@
       <c r="D193" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E193" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F193" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="194" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A194" s="2" t="s">
@@ -5518,12 +4867,6 @@
       <c r="D194" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E194" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F194" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="195" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A195" s="2" t="s">
@@ -5538,12 +4881,6 @@
       <c r="D195" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E195" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F195" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="196" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A196" s="2" t="s">
@@ -5558,12 +4895,6 @@
       <c r="D196" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E196" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F196" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="197" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A197" s="2" t="s">
@@ -5578,12 +4909,6 @@
       <c r="D197" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E197" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F197" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="198" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A198" s="2" t="s">
@@ -5598,12 +4923,6 @@
       <c r="D198" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E198" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F198" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="199" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A199" s="2" t="s">
@@ -5618,12 +4937,6 @@
       <c r="D199" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E199" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F199" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="200" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A200" s="2" t="s">
@@ -5638,12 +4951,6 @@
       <c r="D200" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E200" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F200" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="201" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A201" s="2" t="s">
@@ -5658,12 +4965,6 @@
       <c r="D201" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E201" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F201" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="202" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A202" s="2" t="s">
@@ -5678,12 +4979,6 @@
       <c r="D202" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E202" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F202" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="203" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A203" s="2" t="s">
@@ -5698,12 +4993,6 @@
       <c r="D203" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E203" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F203" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="204" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A204" s="2" t="s">
@@ -5718,12 +5007,6 @@
       <c r="D204" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E204" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F204" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="205" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A205" s="2" t="s">
@@ -5738,12 +5021,6 @@
       <c r="D205" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E205" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F205" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="206" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A206" s="2" t="s">
@@ -5758,12 +5035,6 @@
       <c r="D206" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E206" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F206" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="207" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A207" s="2" t="s">
@@ -5778,12 +5049,6 @@
       <c r="D207" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E207" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F207" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="208" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A208" s="2" t="s">
@@ -5798,12 +5063,6 @@
       <c r="D208" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E208" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F208" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="209" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A209" s="2" t="s">
@@ -5818,12 +5077,6 @@
       <c r="D209" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E209" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F209" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="210" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A210" s="2" t="s">
@@ -5838,12 +5091,6 @@
       <c r="D210" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E210" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F210" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="211" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A211" s="2" t="s">
@@ -5858,12 +5105,6 @@
       <c r="D211" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E211" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F211" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="212" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A212" s="2" t="s">
@@ -5878,12 +5119,6 @@
       <c r="D212" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E212" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F212" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="213" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A213" s="2" t="s">
@@ -5898,12 +5133,6 @@
       <c r="D213" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E213" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F213" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="214" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A214" s="2" t="s">
@@ -5918,12 +5147,6 @@
       <c r="D214" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E214" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F214" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="215" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A215" s="2" t="s">
@@ -5938,12 +5161,6 @@
       <c r="D215" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E215" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F215" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="216" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A216" s="2" t="s">
@@ -5958,12 +5175,6 @@
       <c r="D216" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E216" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F216" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="217" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A217" s="2" t="s">
@@ -5978,12 +5189,6 @@
       <c r="D217" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E217" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F217" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="218" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A218" s="2" t="s">
@@ -5998,12 +5203,6 @@
       <c r="D218" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E218" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F218" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="219" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A219" s="2" t="s">
@@ -6018,12 +5217,6 @@
       <c r="D219" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E219" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F219" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="220" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A220" s="2" t="s">
@@ -6038,12 +5231,6 @@
       <c r="D220" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E220" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F220" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="221" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A221" s="2" t="s">
@@ -6058,12 +5245,6 @@
       <c r="D221" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E221" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F221" t="s" s="0">
-        <v>0</v>
-      </c>
     </row>
     <row r="222" spans="1:1" ht="23.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A222" s="2" t="s">
@@ -6076,12 +5257,6 @@
         <v>0</v>
       </c>
       <c r="D222" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E222" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="F222" t="s" s="0">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
make TA check better
</commit_message>
<xml_diff>
--- a/OOP/src/assets/Book1.xlsx
+++ b/OOP/src/assets/Book1.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5460" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10764" uniqueCount="233">
   <si>
     <t/>
   </si>
@@ -714,6 +714,12 @@
   </si>
   <si>
     <t>ใคร ไม่รู้</t>
+  </si>
+  <si>
+    <t>nong test</t>
+  </si>
+  <si>
+    <t>nong b1</t>
   </si>
 </sst>
 </file>
@@ -1212,19 +1218,19 @@
         <v>10</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>0</v>
+        <v>231</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G4" t="s" s="0">
         <v>0</v>
@@ -1238,19 +1244,19 @@
         <v>11</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>0</v>
+        <v>232</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G5" t="s" s="0">
         <v>0</v>

</xml_diff>